<commit_message>
Made a small correction to FORECAST.ETS.COMPARE
</commit_message>
<xml_diff>
--- a/excel-lambda-walkthrough - FORECAST.ETS.COMPARE (Owen Price - flexyourdata.com).xlsx
+++ b/excel-lambda-walkthrough - FORECAST.ETS.COMPARE (Owen Price - flexyourdata.com).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B6A9CA-38C1-425D-A7F6-24480ED09434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6336D1AC-6564-4BCD-A7A5-F5252692A72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="17640" xr2:uid="{3CF10916-8F3A-45FF-9668-808DB588F900}"/>
   </bookViews>
@@ -3348,7 +3348,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB"/>
-            <a:t>                      IF(ISOMITTED(aggregation),0,aggregation)),</a:t>
+            <a:t>                      IF(ISOMITTED(aggregation),1,aggregation)),</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -8369,7 +8369,7 @@
   <dimension ref="A20:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8940,8 +8940,8 @@
   <sheetPr codeName="Sheet30"/>
   <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="H100" sqref="H100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>